<commit_message>
priprava repo na odevzdani
</commit_message>
<xml_diff>
--- a/smc-table.xlsx
+++ b/smc-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\bakalarska-prace\bakalarska-prace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8399CC-95D8-431C-80FE-BFB68B9BDEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89B34F1-26B8-4531-BB1C-D0C1ACDE26AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -461,7 +461,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>